<commit_message>
Update clr pending bit error
</commit_message>
<xml_diff>
--- a/doc/CAM_CPI_reference.xlsx
+++ b/doc/CAM_CPI_reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Info " sheetId="1" state="visible" r:id="rId2"/>
@@ -645,23 +645,23 @@
 This signal is used also to queue a transfer if one is already ongoing.</t>
   </si>
   <si>
+    <t xml:space="preserve">PENDING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer pending in queue status flag:
+-1'b0: free
+-1'b1: pending</t>
+  </si>
+  <si>
     <t xml:space="preserve">CLR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W</t>
   </si>
   <si>
     <t xml:space="preserve">Channel clear and stop transfer:
 -1'b0: disable
 -1'b1: enable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PENDING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transfer pending in queue status flag:
--1'b0: free
--1'b1: pending</t>
   </si>
   <si>
     <t xml:space="preserve">FRAMEDROP_EN</t>
@@ -771,7 +771,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -793,87 +793,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -906,54 +825,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF666699"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -970,31 +847,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC3D69B"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -1082,7 +944,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1106,54 +968,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1164,135 +978,135 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1304,11 +1118,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1316,99 +1130,99 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="2" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="10" xfId="36" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="10" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="10" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="10" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="10" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1432,50 +1246,34 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="36" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF77933C"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC3D69B"/>
@@ -1487,7 +1285,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1503,7 +1301,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1511,7 +1309,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF77933C"/>
+      <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -1532,16 +1330,16 @@
   </sheetPr>
   <dimension ref="B1:D28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="40.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="11.42"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="40.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1771,7 +1569,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1786,17 +1584,17 @@
   </sheetPr>
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="22.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="23.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="43.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="30.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="23" width="10.58"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="23.219387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="42.7908163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="23" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2115,7 +1913,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2130,19 +1928,19 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="45.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="44" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="44" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="44" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="8" style="23" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="10.58"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="44" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="45.2244897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="44" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="44" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="44" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="23" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2185,7 +1983,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2200,22 +1998,22 @@
   </sheetPr>
   <dimension ref="A1:AMC27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="23" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="23" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="23" width="12.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="23" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="23" width="10.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="16" style="23" width="9.13"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="22" style="23" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1017" min="23" style="23" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1018" style="0" width="9.13"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="2" style="23" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="23" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="23" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="23" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="23" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="21" min="16" style="23" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="23" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1017" min="23" style="23" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="9.04591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3647,7 +3445,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3662,23 +3460,23 @@
   </sheetPr>
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="54" width="19.85"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="54" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="55" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="55" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="55" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="24" width="70.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="54" width="19.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="54" width="9.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="54" width="9.13"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="54" width="19.5714285714286"/>
+    <col collapsed="false" hidden="true" max="2" min="2" style="54" width="0"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="55" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="55" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="55" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="24" width="69.9234693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="54" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="54" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="54" width="9.04591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4063,7 +3861,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4076,25 +3874,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+      <selection pane="bottomLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="59" width="18.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="12.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="44" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="44" width="16.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="44" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="60" width="56.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="61" width="9.13"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="59" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="44" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="44" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="44" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="44" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="60" width="56.1581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="61" width="9.04591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4267,10 +4065,10 @@
         <v>1</v>
       </c>
       <c r="E7" s="55" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7" s="64" t="s">
         <v>186</v>
-      </c>
-      <c r="F7" s="64" t="s">
-        <v>158</v>
       </c>
       <c r="G7" s="65" t="s">
         <v>135</v>
@@ -4279,7 +4077,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="63" t="s">
         <v>188</v>
       </c>
@@ -4287,16 +4085,16 @@
         <v>142</v>
       </c>
       <c r="C8" s="64" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8" s="64" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="55" t="s">
+        <v>186</v>
+      </c>
+      <c r="F8" s="64" t="s">
         <v>158</v>
-      </c>
-      <c r="F8" s="64" t="s">
-        <v>186</v>
       </c>
       <c r="G8" s="65" t="s">
         <v>135</v>
@@ -4799,10 +4597,11 @@
         <v>216</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4817,23 +4616,23 @@
   </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="61" width="19.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="61" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="44" width="17.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="44" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="44" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="60" width="31.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="61" width="9.13"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="61" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="61" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="44" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="44" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="44" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="44" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="60" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="61" width="9.04591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4865,7 +4664,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4880,17 +4679,17 @@
   </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.54"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4910,7 +4709,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Fix UDMA : clr to bit 6, pending to bit 5
</commit_message>
<xml_diff>
--- a/doc/CAM_CPI_reference.xlsx
+++ b/doc/CAM_CPI_reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Info " sheetId="1" state="visible" r:id="rId2"/>
@@ -645,23 +645,23 @@
 This signal is used also to queue a transfer if one is already ongoing.</t>
   </si>
   <si>
+    <t xml:space="preserve">PENDING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer pending in queue status flag:
+-1'b0: free
+-1'b1: pending</t>
+  </si>
+  <si>
     <t xml:space="preserve">CLR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W</t>
   </si>
   <si>
     <t xml:space="preserve">Channel clear and stop transfer:
 -1'b0: disable
 -1'b1: enable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PENDING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transfer pending in queue status flag:
--1'b0: free
--1'b1: pending</t>
   </si>
   <si>
     <t xml:space="preserve">FRAMEDROP_EN</t>
@@ -771,7 +771,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -793,87 +793,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -906,54 +825,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF666699"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -970,31 +847,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC3D69B"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -1082,7 +944,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1106,54 +968,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1164,135 +978,135 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1304,11 +1118,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1316,99 +1130,99 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="2" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="10" xfId="36" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="10" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="10" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="10" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="10" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1432,50 +1246,34 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="36" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF77933C"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC3D69B"/>
@@ -1487,7 +1285,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1503,7 +1301,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1511,7 +1309,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF77933C"/>
+      <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -1532,16 +1330,16 @@
   </sheetPr>
   <dimension ref="B1:D28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="40.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="11.42"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="40.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1771,7 +1569,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1786,17 +1584,17 @@
   </sheetPr>
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="22.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="23.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="43.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="30.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="23" width="10.58"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="23.219387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="42.7908163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="23" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2115,7 +1913,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2130,19 +1928,19 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="45.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="44" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="44" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="44" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="8" style="23" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="10.58"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="44" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="45.2244897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="44" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="44" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="44" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="23" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2185,7 +1983,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2200,22 +1998,22 @@
   </sheetPr>
   <dimension ref="A1:AMC27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="23" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="23" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="23" width="12.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="23" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="23" width="10.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="16" style="23" width="9.13"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="22" style="23" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1017" min="23" style="23" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1018" style="0" width="9.13"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="2" style="23" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="23" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="23" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="23" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="23" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="21" min="16" style="23" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="23" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1017" min="23" style="23" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="9.04591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3647,7 +3445,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3662,23 +3460,23 @@
   </sheetPr>
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="54" width="19.85"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="54" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="55" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="55" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="55" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="24" width="70.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="54" width="19.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="54" width="9.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="54" width="9.13"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="54" width="19.5714285714286"/>
+    <col collapsed="false" hidden="true" max="2" min="2" style="54" width="0"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="55" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="55" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="55" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="24" width="69.9234693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="54" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="54" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="54" width="9.04591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4063,7 +3861,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4076,25 +3874,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="59" width="18.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="12.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="44" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="44" width="16.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="44" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="60" width="56.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="61" width="9.13"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="59" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="44" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="44" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="44" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="44" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="60" width="56.1581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="61" width="9.04591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4267,10 +4065,10 @@
         <v>1</v>
       </c>
       <c r="E7" s="55" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7" s="64" t="s">
         <v>186</v>
-      </c>
-      <c r="F7" s="64" t="s">
-        <v>158</v>
       </c>
       <c r="G7" s="65" t="s">
         <v>135</v>
@@ -4279,7 +4077,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="63" t="s">
         <v>188</v>
       </c>
@@ -4287,16 +4085,16 @@
         <v>142</v>
       </c>
       <c r="C8" s="64" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8" s="64" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="55" t="s">
+        <v>186</v>
+      </c>
+      <c r="F8" s="64" t="s">
         <v>158</v>
-      </c>
-      <c r="F8" s="64" t="s">
-        <v>186</v>
       </c>
       <c r="G8" s="65" t="s">
         <v>135</v>
@@ -4799,10 +4597,11 @@
         <v>216</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4817,23 +4616,23 @@
   </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="61" width="19.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="61" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="44" width="17.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="44" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="44" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="60" width="31.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="61" width="9.13"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="61" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="61" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="44" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="44" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="44" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="44" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="60" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="61" width="9.04591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4865,7 +4664,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4880,17 +4679,17 @@
   </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.54"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4910,7 +4709,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>